<commit_message>
add change color & font size
</commit_message>
<xml_diff>
--- a/file/my-kpi.xlsx
+++ b/file/my-kpi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KPI-Tracker\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4323B2BA-6FF3-47D9-9737-64A02E247749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D71B9BC-6A3E-4E20-8DEC-798626539245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <t>Số giờ mục tiêu*</t>
   </si>
   <si>
-    <t>Cá nhân</t>
+    <t>Học tập</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,7 +421,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add kpi info popup
</commit_message>
<xml_diff>
--- a/file/my-kpi.xlsx
+++ b/file/my-kpi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KPI-Tracker\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D71B9BC-6A3E-4E20-8DEC-798626539245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1886CEA2-6DCF-4FC9-8BD4-B015038CB6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Tên chỉ tiêu*</t>
   </si>
@@ -36,7 +36,10 @@
     <t>Số giờ mục tiêu*</t>
   </si>
   <si>
-    <t>Học tập</t>
+    <t>Lao động</t>
+  </si>
+  <si>
+    <t>#000080</t>
   </si>
 </sst>
 </file>
@@ -397,7 +400,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,6 +423,9 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="C2" s="1">
         <v>70</v>
       </c>

</xml_diff>